<commit_message>
added new branch mod-schedule
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>Firstname</t>
   </si>
@@ -100,6 +100,27 @@
   </si>
   <si>
     <t>sad</t>
+  </si>
+  <si>
+    <t>sadas</t>
+  </si>
+  <si>
+    <t>sa</t>
+  </si>
+  <si>
+    <t>Won</t>
+  </si>
+  <si>
+    <t>Lyon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEW </t>
+  </si>
+  <si>
+    <t>oLd</t>
+  </si>
+  <si>
+    <t>asdas</t>
   </si>
 </sst>
 </file>
@@ -467,11 +488,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,6 +623,77 @@
       </c>
       <c r="L3" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>123123</v>
+      </c>
+      <c r="K5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6">
+        <v>3123</v>
+      </c>
+      <c r="G6">
+        <v>123</v>
+      </c>
+      <c r="H6">
+        <v>123</v>
+      </c>
+      <c r="K6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7">
+        <v>24352435</v>
+      </c>
+      <c r="K7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>